<commit_message>
Update frontend V 2
</commit_message>
<xml_diff>
--- a/src/assets/excel/RUMUS PAKAR DEMPSTER SHAFER SKRIPSI.xlsx
+++ b/src/assets/excel/RUMUS PAKAR DEMPSTER SHAFER SKRIPSI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ptikum1-my.sharepoint.com/personal/gabriel_arta_1903126_students_um_ac_id/Documents/~KULIAH S1 MTK/sempro/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ptikum1-my.sharepoint.com/personal/gabriel_arta_1903126_students_um_ac_id/Documents/~KULIAH S1 MTK/SEM 8/SKRIPSI/SISTEM-PAKAR-DEMPSTER-SHAFER/frontend/src/assets/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{87629D1B-EE53-4B63-8F86-B221D3F26A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{015C96EB-09E3-4F1C-B6B7-72870437B693}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{87629D1B-EE53-4B63-8F86-B221D3F26A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12FAFFC4-831D-4051-BE06-9C3581A55BE9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{D00C754F-CDEE-4336-A39A-B15390190D59}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{D00C754F-CDEE-4336-A39A-B15390190D59}"/>
   </bookViews>
   <sheets>
     <sheet name="PAKAR 1 - arbin janu" sheetId="3" r:id="rId1"/>
@@ -155,9 +155,6 @@
     <t>m1{A,E,F,H,M}</t>
   </si>
   <si>
-    <t>m2{B,C,D,E}</t>
-  </si>
-  <si>
     <t>m3{N}</t>
   </si>
   <si>
@@ -182,24 +179,15 @@
     <t>AEFHM</t>
   </si>
   <si>
-    <t>BCDE</t>
-  </si>
-  <si>
     <t>m10{E}</t>
   </si>
   <si>
     <t>M10{AEFHM}</t>
   </si>
   <si>
-    <t>m10{BCDE}</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
-    <t>m11{BCDE}</t>
-  </si>
-  <si>
     <t>M11{AEFHM}</t>
   </si>
   <si>
@@ -215,9 +203,6 @@
     <t>M12{AEFHM}</t>
   </si>
   <si>
-    <t>m12{BCDE}</t>
-  </si>
-  <si>
     <t>m12{E}</t>
   </si>
   <si>
@@ -242,9 +227,6 @@
     <t>M13{AEFHM}</t>
   </si>
   <si>
-    <t>m13{BCDE}</t>
-  </si>
-  <si>
     <t>m13{N}</t>
   </si>
   <si>
@@ -260,9 +242,6 @@
     <t>M14{AEFHM}</t>
   </si>
   <si>
-    <t>m14{BCDE}</t>
-  </si>
-  <si>
     <t>m14{N}</t>
   </si>
   <si>
@@ -287,9 +266,6 @@
     <t>M15{AEFHM}</t>
   </si>
   <si>
-    <t>m15{BCDE}</t>
-  </si>
-  <si>
     <t>m15{N}</t>
   </si>
   <si>
@@ -329,9 +305,6 @@
     <t>m16{N}</t>
   </si>
   <si>
-    <t>m16{BCDE}</t>
-  </si>
-  <si>
     <t>M16{AEFHM}</t>
   </si>
   <si>
@@ -359,9 +332,6 @@
     <t>m17{N}</t>
   </si>
   <si>
-    <t>m17{BCDE}</t>
-  </si>
-  <si>
     <t>M17{AEFHM}</t>
   </si>
   <si>
@@ -597,6 +567,36 @@
   </si>
   <si>
     <t>m15{CDGIJK}</t>
+  </si>
+  <si>
+    <t>m2{B,C,D,E,J}</t>
+  </si>
+  <si>
+    <t>m10{BCDEJ}</t>
+  </si>
+  <si>
+    <t>m12{BCDEJ}</t>
+  </si>
+  <si>
+    <t>BCDEJ</t>
+  </si>
+  <si>
+    <t>m14{BCDEJ}</t>
+  </si>
+  <si>
+    <t>m11{BCDEJ}</t>
+  </si>
+  <si>
+    <t>m16{BCDEJ}</t>
+  </si>
+  <si>
+    <t>m13{BCDEJ}</t>
+  </si>
+  <si>
+    <t>m15{BCDEJ}</t>
+  </si>
+  <si>
+    <t>m17{BCDEJ}</t>
   </si>
 </sst>
 </file>
@@ -1073,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2747943-B627-4176-8D1F-11B5E0FF2B7C}">
   <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="E13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1115,13 +1115,13 @@
         <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="K1" t="s">
         <v>17</v>
       </c>
       <c r="L1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -1146,13 +1146,13 @@
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="K2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="L2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -1160,7 +1160,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>173</v>
       </c>
       <c r="C3" s="17">
         <f t="shared" ref="C3:C10" si="0">E3/$E$1</f>
@@ -1177,13 +1177,13 @@
         <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K3" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="L3" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -1191,7 +1191,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="17">
         <f t="shared" si="0"/>
@@ -1208,13 +1208,13 @@
         <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="K4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="L4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -1222,7 +1222,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="17">
         <f t="shared" si="0"/>
@@ -1239,13 +1239,13 @@
         <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="K5" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="L5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
@@ -1253,7 +1253,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="17">
         <f t="shared" si="0"/>
@@ -1270,13 +1270,13 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="K6" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="L6" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
@@ -1284,7 +1284,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="17">
         <f t="shared" si="0"/>
@@ -1301,13 +1301,13 @@
         <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="K7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L7" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
@@ -1315,7 +1315,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="17">
         <f t="shared" si="0"/>
@@ -1334,7 +1334,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="17">
         <f t="shared" si="0"/>
@@ -1353,7 +1353,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="17">
         <f t="shared" si="0"/>
@@ -1371,13 +1371,13 @@
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>23</v>
       </c>
       <c r="I12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>23</v>
@@ -1389,7 +1389,7 @@
         <v>23</v>
       </c>
       <c r="S12" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="T12" s="19" t="s">
         <v>23</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="20">
         <f>C2</f>
@@ -1459,7 +1459,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H14" s="6">
         <f>D28</f>
@@ -1474,7 +1474,7 @@
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="L14" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M14" s="9">
         <f>I41</f>
@@ -1489,7 +1489,7 @@
         <v>1.1291779584462513E-2</v>
       </c>
       <c r="Q14" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R14" s="9">
         <f>N51</f>
@@ -1521,7 +1521,7 @@
         <v>0.1875</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
       <c r="H15" s="6">
         <f>D29</f>
@@ -1536,7 +1536,7 @@
         <v>0.15</v>
       </c>
       <c r="L15" s="19" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
       <c r="M15" s="9">
         <f>I42</f>
@@ -1551,7 +1551,7 @@
         <v>0.10162601626016259</v>
       </c>
       <c r="Q15" s="19" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
       <c r="R15" s="9">
         <f>N50</f>
@@ -1568,7 +1568,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16" s="18">
         <f>D14/1</f>
@@ -1622,14 +1622,14 @@
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="18">
         <f>E14/1</f>
         <v>6.25E-2</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H17" s="6">
         <f>D31</f>
@@ -1644,7 +1644,7 @@
         <v>0.15</v>
       </c>
       <c r="L17" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M17" s="9">
         <f>I43</f>
@@ -1659,7 +1659,7 @@
         <v>0.10162601626016259</v>
       </c>
       <c r="Q17" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="R17" s="9">
         <f>N49</f>
@@ -1676,7 +1676,7 @@
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>47</v>
+        <v>174</v>
       </c>
       <c r="D18" s="18">
         <f>D15/1</f>
@@ -1698,7 +1698,7 @@
         <v>4.9999999999999996E-2</v>
       </c>
       <c r="L18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="M18" s="9">
         <f>I44</f>
@@ -1713,7 +1713,7 @@
         <v>4.7425474254742556E-2</v>
       </c>
       <c r="Q18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="R18" s="9">
         <f>N52</f>
@@ -1737,7 +1737,7 @@
         <v>0.1875</v>
       </c>
       <c r="L19" s="19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="M19" s="9">
         <f>I45</f>
@@ -1752,7 +1752,7 @@
         <v>0.14227642276422764</v>
       </c>
       <c r="Q19" s="19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="R19" s="9">
         <f>N53</f>
@@ -1773,14 +1773,14 @@
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I20" s="14">
         <f>I15/(1-(I14+I16+I17))</f>
         <v>0.30143540669856461</v>
       </c>
       <c r="L20" s="19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M20" s="9">
         <f>I46</f>
@@ -1795,7 +1795,7 @@
         <v>6.7750677506775062E-2</v>
       </c>
       <c r="Q20" s="19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="R20" s="9">
         <f>N54</f>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.3">
       <c r="H21" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I21" s="14">
         <f>J14/(1-(I14+I16+I17))</f>
@@ -1852,21 +1852,21 @@
     <row r="22" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C22" s="19"/>
       <c r="D22" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>23</v>
       </c>
       <c r="F22" s="19"/>
       <c r="H22" t="s">
-        <v>55</v>
+        <v>175</v>
       </c>
       <c r="I22" s="14">
         <f>J15/(1-(I14+I16+I17))</f>
         <v>0.21531100478468898</v>
       </c>
       <c r="Q22" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="R22" s="9">
         <f>N47</f>
@@ -1895,21 +1895,21 @@
       </c>
       <c r="F23" s="19"/>
       <c r="H23" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I23" s="14">
         <f>J16/(1-(I14+I16+I17))</f>
         <v>7.1770334928229665E-2</v>
       </c>
       <c r="M23" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="N23" s="23">
         <f>(N15+N16+N20+O16)/(1-(N17+N18+N19))</f>
         <v>0.4532374100719424</v>
       </c>
       <c r="Q23" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="R23" s="9">
         <f>N56</f>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B24" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="20">
         <f>D17</f>
@@ -1942,14 +1942,14 @@
       </c>
       <c r="F24" s="19"/>
       <c r="H24" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I24" s="14">
         <f>J17/(1-(I14+I16+I17))</f>
         <v>0.21531100478468898</v>
       </c>
       <c r="M24" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="N24" s="23">
         <f>O14/(1-(N17+N18+N19))</f>
@@ -1973,7 +1973,7 @@
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B25" s="19" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
       <c r="C25" s="20">
         <f>D18</f>
@@ -1989,14 +1989,14 @@
       </c>
       <c r="F25" s="19"/>
       <c r="H25" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I25" s="14">
         <f>I18/(1-(I14+I16+I17))</f>
         <v>0.10047846889952154</v>
       </c>
       <c r="M25" t="s">
-        <v>70</v>
+        <v>177</v>
       </c>
       <c r="N25" s="23">
         <f>O15/(1-(N17+N18+N19))</f>
@@ -2028,14 +2028,14 @@
         <v>7.1770334928229665E-2</v>
       </c>
       <c r="M26" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="N26" s="23">
         <f>O17/(1-(N17+N18+N19))</f>
         <v>0.10791366906474818</v>
       </c>
       <c r="R26" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="S26" s="23">
         <f>(S14+S22+S23+S24)/(1-(SUM(S15:S21)))</f>
@@ -2064,14 +2064,14 @@
         <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="N27" s="23">
         <f>O18/(1-(N17+N18+N19))</f>
         <v>5.035971223021584E-2</v>
       </c>
       <c r="R27" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="S27" s="23">
         <f>T22/(1-(SUM(S15:S21)))</f>
@@ -2081,7 +2081,7 @@
     <row r="28" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B28" s="19"/>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D28" s="18">
         <f>E24/(1-(D24+D25+D26))</f>
@@ -2090,14 +2090,14 @@
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="M28" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="N28" s="23">
         <f>O19/(1-(N17+N18+N19))</f>
         <v>0.15107913669064749</v>
       </c>
       <c r="R28" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="S28" s="23">
         <f>T16/(1-(SUM(S15:S21)))</f>
@@ -2106,21 +2106,21 @@
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>49</v>
+        <v>178</v>
       </c>
       <c r="D29" s="18">
         <f>E25/(1-(D24+D25+D26))</f>
         <v>0.36</v>
       </c>
       <c r="M29" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="N29" s="23">
         <f>O20/(1-(N17+N18+N19))</f>
         <v>7.1942446043165464E-2</v>
       </c>
       <c r="R29" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S29" s="23">
         <f>T17/(1-(SUM(S15:S21)))</f>
@@ -2136,20 +2136,20 @@
         <v>0.12</v>
       </c>
       <c r="I30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J30" s="19" t="s">
         <v>23</v>
       </c>
       <c r="M30" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="N30" s="23">
         <f>(N21+N14)/(1-(N17+N18+N19))</f>
         <v>9.5923261390887284E-3</v>
       </c>
       <c r="R30" t="s">
-        <v>93</v>
+        <v>179</v>
       </c>
       <c r="S30" s="23">
         <f>T15/(1-(SUM(S15:S21)))</f>
@@ -2158,7 +2158,7 @@
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D31" s="18">
         <f>D27/(1-(D24+D25+D26))</f>
@@ -2183,7 +2183,7 @@
         <v>3.5971223021582739E-2</v>
       </c>
       <c r="R31" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="S31" s="23">
         <f>T14/(1-(SUM(S15:S21)))</f>
@@ -2199,7 +2199,7 @@
         <v>0.12</v>
       </c>
       <c r="G32" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H32" s="6">
         <f>I21</f>
@@ -2218,7 +2218,7 @@
         <v>0.99999999999999989</v>
       </c>
       <c r="R32" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="S32" s="23">
         <f>T18/(1-(SUM(S15:S21)))</f>
@@ -2231,7 +2231,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="19" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
       <c r="H33" s="6">
         <f>I22</f>
@@ -2246,7 +2246,7 @@
         <v>7.1770334928229665E-2</v>
       </c>
       <c r="R33" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="S33" s="23">
         <f>T19/(1-(SUM(S15:S21)))</f>
@@ -2270,7 +2270,7 @@
         <v>2.3923444976076558E-2</v>
       </c>
       <c r="R34" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="S34" s="23">
         <f>T20/(1-(SUM(S15:S21)))</f>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="35" spans="4:20" x14ac:dyDescent="0.3">
       <c r="G35" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H35" s="6">
         <f>I24</f>
@@ -2294,13 +2294,13 @@
         <v>7.1770334928229665E-2</v>
       </c>
       <c r="N35" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="O35" s="19" t="s">
         <v>23</v>
       </c>
       <c r="R35" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="S35" s="23">
         <f>T21/(1-(SUM(S15:S21)))</f>
@@ -2309,7 +2309,7 @@
     </row>
     <row r="36" spans="4:20" x14ac:dyDescent="0.3">
       <c r="G36" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H36" s="6">
         <f>I25</f>
@@ -2335,7 +2335,7 @@
         <v>0.58333333333333326</v>
       </c>
       <c r="R36" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="S36" s="23">
         <f>T23/(1-(SUM(S15:S21)))</f>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="37" spans="4:20" x14ac:dyDescent="0.3">
       <c r="G37" s="19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H37" s="6">
         <f>I20</f>
@@ -2359,7 +2359,7 @@
         <v>0.10047846889952154</v>
       </c>
       <c r="L37" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M37" s="9">
         <f>N24</f>
@@ -2398,7 +2398,7 @@
         <v>2.3923444976076558E-2</v>
       </c>
       <c r="L38" s="19" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
       <c r="M38" s="9">
         <f>N25</f>
@@ -2436,14 +2436,14 @@
     </row>
     <row r="40" spans="4:20" x14ac:dyDescent="0.3">
       <c r="H40" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I40" s="27">
         <f>(I32+I33+I34+J34)/(1-(I35+I36+I37))</f>
         <v>0.39295392953929531</v>
       </c>
       <c r="L40" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M40" s="9">
         <f t="shared" ref="M40:M45" si="10">N26</f>
@@ -2467,14 +2467,14 @@
     </row>
     <row r="41" spans="4:20" x14ac:dyDescent="0.3">
       <c r="H41" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I41">
         <f>J32/(1-(I35+I36+I37))</f>
         <v>1.3550135501355014E-2</v>
       </c>
       <c r="L41" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="M41" s="9">
         <f t="shared" si="10"/>
@@ -2502,14 +2502,14 @@
     </row>
     <row r="42" spans="4:20" x14ac:dyDescent="0.3">
       <c r="H42" t="s">
-        <v>64</v>
+        <v>180</v>
       </c>
       <c r="I42">
         <f>J33/(1-(I35+I36+I37))</f>
         <v>0.12195121951219511</v>
       </c>
       <c r="L42" s="19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="M42" s="9">
         <f t="shared" si="10"/>
@@ -2524,7 +2524,7 @@
         <v>8.8129496402877691E-2</v>
       </c>
       <c r="Q42" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R42" s="26">
         <f>S31</f>
@@ -2541,14 +2541,14 @@
     </row>
     <row r="43" spans="4:20" x14ac:dyDescent="0.3">
       <c r="H43" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I43">
         <f>J35/(1-(I35+I36+I37))</f>
         <v>0.12195121951219511</v>
       </c>
       <c r="L43" s="19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M43" s="9">
         <f t="shared" si="10"/>
@@ -2563,7 +2563,7 @@
         <v>4.1966426858513185E-2</v>
       </c>
       <c r="Q43" s="7" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
       <c r="R43" s="26">
         <f>S30</f>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="44" spans="4:20" x14ac:dyDescent="0.3">
       <c r="H44" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I44" s="5">
         <f>J36/(1-(SUM(I35:I37)))</f>
@@ -2619,7 +2619,7 @@
     </row>
     <row r="45" spans="4:20" x14ac:dyDescent="0.3">
       <c r="H45" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I45">
         <f>J37/(1-(I35+I36+I37))</f>
@@ -2641,7 +2641,7 @@
         <v>2.0983213429256596E-2</v>
       </c>
       <c r="Q45" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="R45" s="26">
         <f>S29</f>
@@ -2658,14 +2658,14 @@
     </row>
     <row r="46" spans="4:20" x14ac:dyDescent="0.3">
       <c r="H46" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I46">
         <f>I38/(1-(I35+I36+I37))</f>
         <v>8.1300813008130066E-2</v>
       </c>
       <c r="Q46" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="R46" s="26">
         <f>S32</f>
@@ -2689,14 +2689,14 @@
         <v>4.065040650406504E-2</v>
       </c>
       <c r="M47" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="N47" s="5">
         <f>N37/(1-(N41+N42))</f>
         <v>5.4537521815008743E-3</v>
       </c>
       <c r="Q47" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="R47" s="26">
         <f>S33</f>
@@ -2717,14 +2717,14 @@
         <v>0.99999999999999989</v>
       </c>
       <c r="M48" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="N48" s="5">
         <f>(N38+N39+O39+N43)/(1-(N41+N42))</f>
         <v>0.57657068062827221</v>
       </c>
       <c r="Q48" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="R48" s="26">
         <f>S34</f>
@@ -2741,7 +2741,7 @@
     </row>
     <row r="49" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M49" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="N49" s="5">
         <f>(N40+O40)/(1-(N41+N42))</f>
@@ -2765,14 +2765,14 @@
     </row>
     <row r="50" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M50" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="N50" s="5">
         <f>O38/(1-(N41+N42))</f>
         <v>6.8717277486910977E-2</v>
       </c>
       <c r="Q50" s="7" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="R50" s="26">
         <f>S27</f>
@@ -2789,14 +2789,14 @@
     </row>
     <row r="51" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M51" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="N51" s="5">
         <f>O37/(1-(N41+N42))</f>
         <v>7.6352530541012225E-3</v>
       </c>
       <c r="Q51" s="7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="R51" s="26">
         <f>S36</f>
@@ -2813,14 +2813,14 @@
     </row>
     <row r="52" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M52" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="N52" s="5">
         <f>O41/(1-(N41+N42))</f>
         <v>3.2068062827225137E-2</v>
       </c>
       <c r="Q52" s="7" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="R52" s="26">
         <f>S26</f>
@@ -2837,7 +2837,7 @@
     </row>
     <row r="53" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M53" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="N53" s="5">
         <f>O42/(1-(N41+N42))</f>
@@ -2861,7 +2861,7 @@
     </row>
     <row r="54" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M54" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="N54" s="5">
         <f>O43/(1-(N41+N42))</f>
@@ -2870,7 +2870,7 @@
     </row>
     <row r="55" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M55" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="N55" s="5">
         <f>(N44+O44)/(1-(N41+N42))</f>
@@ -2887,14 +2887,14 @@
     </row>
     <row r="56" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M56" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="N56" s="5">
         <f>N45/(1-(N41+N42))</f>
         <v>1.6361256544502621E-2</v>
       </c>
       <c r="R56" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="S56">
         <f>T52/(1-(SUM(S43:S48)+S52))</f>
@@ -2911,7 +2911,7 @@
         <v>2.2905759162303668E-2</v>
       </c>
       <c r="R57" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="S57">
         <f>T50/(1-(SUM(S43:S48)+S52))</f>
@@ -2935,7 +2935,7 @@
     </row>
     <row r="59" spans="13:20" x14ac:dyDescent="0.3">
       <c r="R59" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="S59">
         <f>T45/(1-(SUM(S43:S48)+S52))</f>
@@ -2945,7 +2945,7 @@
     </row>
     <row r="60" spans="13:20" x14ac:dyDescent="0.3">
       <c r="R60" t="s">
-        <v>103</v>
+        <v>182</v>
       </c>
       <c r="S60">
         <f>T43/(1-(SUM(S43:S48)+S52))</f>
@@ -2955,7 +2955,7 @@
     </row>
     <row r="61" spans="13:20" x14ac:dyDescent="0.3">
       <c r="R61" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="S61">
         <f>T42/(1-(SUM(S43:S48)+S52))</f>
@@ -2965,7 +2965,7 @@
     </row>
     <row r="62" spans="13:20" x14ac:dyDescent="0.3">
       <c r="R62" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="S62">
         <f>T46/(1-(SUM(S43:S48)+S52))</f>
@@ -2975,7 +2975,7 @@
     </row>
     <row r="63" spans="13:20" x14ac:dyDescent="0.3">
       <c r="R63" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="S63">
         <f>T47/(1-(SUM(S43:S48)+S52))</f>
@@ -2985,7 +2985,7 @@
     </row>
     <row r="64" spans="13:20" x14ac:dyDescent="0.3">
       <c r="R64" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="S64">
         <f>T48/(1-(SUM(S43:S48)+S52))</f>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="66" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R66" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="S66">
         <f>T51/(1-(SUM(S43:S48)+S52))</f>
@@ -3042,7 +3042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC07727-2819-4CB1-89A4-19B568562B93}">
   <dimension ref="A1:U67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K1" sqref="K1:L7"/>
     </sheetView>
   </sheetViews>
@@ -3085,13 +3085,13 @@
         <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="K1" t="s">
         <v>17</v>
       </c>
       <c r="L1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -3099,7 +3099,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C2" s="17">
         <f>E2/$E$1</f>
@@ -3116,13 +3116,13 @@
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="K2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="L2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -3130,7 +3130,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C3" s="17">
         <f t="shared" ref="C3:C10" si="0">E3/$E$1</f>
@@ -3147,13 +3147,13 @@
         <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K3" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="L3" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -3161,7 +3161,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="17">
         <f t="shared" si="0"/>
@@ -3178,13 +3178,13 @@
         <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="K4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="L4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -3192,7 +3192,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C5" s="17">
         <f t="shared" si="0"/>
@@ -3209,13 +3209,13 @@
         <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="K5" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="L5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
@@ -3223,7 +3223,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C6" s="17">
         <f t="shared" si="0"/>
@@ -3240,13 +3240,13 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="K6" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="L6" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
@@ -3254,7 +3254,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="17">
         <f t="shared" si="0"/>
@@ -3271,13 +3271,13 @@
         <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="K7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L7" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
@@ -3285,7 +3285,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C8" s="17">
         <f t="shared" si="0"/>
@@ -3304,7 +3304,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C9" s="17">
         <f t="shared" si="0"/>
@@ -3323,7 +3323,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C10" s="17">
         <f t="shared" si="0"/>
@@ -3341,13 +3341,13 @@
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>23</v>
       </c>
       <c r="I12" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>23</v>
@@ -3359,7 +3359,7 @@
         <v>23</v>
       </c>
       <c r="S12" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="T12" s="19" t="s">
         <v>23</v>
@@ -3414,7 +3414,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C14" s="20">
         <f>C2</f>
@@ -3429,7 +3429,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="H14" s="6">
         <f>D28</f>
@@ -3444,7 +3444,7 @@
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="L14" s="19" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="M14" s="9">
         <f>I40</f>
@@ -3459,7 +3459,7 @@
         <v>1.2664640324214793E-2</v>
       </c>
       <c r="Q14" s="19" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="R14" s="9">
         <f>N53</f>
@@ -3491,7 +3491,7 @@
         <v>0.1875</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="H15" s="6">
         <f>D29</f>
@@ -3506,7 +3506,7 @@
         <v>0.15</v>
       </c>
       <c r="L15" s="19" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="M15" s="9">
         <f>I41</f>
@@ -3521,7 +3521,7 @@
         <v>0.11398176291793313</v>
       </c>
       <c r="Q15" s="19" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="R15" s="9">
         <f>N54</f>
@@ -3538,7 +3538,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16" s="18">
         <f>D14/1</f>
@@ -3592,14 +3592,14 @@
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D17" s="18">
         <f>E14/1</f>
         <v>6.25E-2</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H17" s="6">
         <f>D31</f>
@@ -3614,7 +3614,7 @@
         <v>0.15</v>
       </c>
       <c r="L17" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M17" s="9">
         <f t="shared" si="6"/>
@@ -3629,7 +3629,7 @@
         <v>0.34194528875379931</v>
       </c>
       <c r="Q17" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="R17" s="9">
         <f>N55</f>
@@ -3646,7 +3646,7 @@
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D18" s="18">
         <f>D15/1</f>
@@ -3668,7 +3668,7 @@
         <v>4.9999999999999996E-2</v>
       </c>
       <c r="L18" s="19" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="M18" s="9">
         <f t="shared" si="6"/>
@@ -3683,7 +3683,7 @@
         <v>0.15957446808510639</v>
       </c>
       <c r="Q18" s="19" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="R18" s="9">
         <f>N56</f>
@@ -3707,7 +3707,7 @@
         <v>0.1875</v>
       </c>
       <c r="L19" s="19" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="M19" s="9">
         <f t="shared" si="6"/>
@@ -3722,7 +3722,7 @@
         <v>5.3191489361702135E-2</v>
       </c>
       <c r="Q19" s="19" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="R19" s="9">
         <f>N57</f>
@@ -3743,14 +3743,14 @@
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="I20" s="14">
         <f>I15/(1-(I14+I16+I17))</f>
         <v>0.30143540669856461</v>
       </c>
       <c r="L20" s="19" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="M20" s="9">
         <f t="shared" si="6"/>
@@ -3765,7 +3765,7 @@
         <v>7.598784194528875E-2</v>
       </c>
       <c r="Q20" s="19" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="R20" s="9">
         <f>N58</f>
@@ -3782,7 +3782,7 @@
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.3">
       <c r="H21" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="I21" s="14">
         <f>J14/(1-(I14+I16+I17))</f>
@@ -3804,7 +3804,7 @@
         <v>3.7993920972644382E-2</v>
       </c>
       <c r="Q21" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="R21" s="9">
         <f>N59</f>
@@ -3822,14 +3822,14 @@
     <row r="22" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C22" s="19"/>
       <c r="D22" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>23</v>
       </c>
       <c r="F22" s="19"/>
       <c r="H22" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="I22" s="14">
         <f>J15/(1-(I14+I16+I17))</f>
@@ -3865,21 +3865,21 @@
       </c>
       <c r="F23" s="19"/>
       <c r="H23" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I23" s="14">
         <f>J16/(1-(I14+I16+I17))</f>
         <v>7.1770334928229665E-2</v>
       </c>
       <c r="M23" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="N23" s="23">
         <f>(N15+N16+O16)/(1-(SUM(N17:N20)))</f>
         <v>7.8260869565217384E-2</v>
       </c>
       <c r="Q23" s="19" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="R23" s="9">
         <f>N47</f>
@@ -3896,7 +3896,7 @@
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B24" s="19" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C24" s="20">
         <f>D17</f>
@@ -3912,21 +3912,21 @@
       </c>
       <c r="F24" s="19"/>
       <c r="H24" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I24" s="14">
         <f>J17/(1-(I14+I16+I17))</f>
         <v>0.21531100478468898</v>
       </c>
       <c r="M24" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="N24" s="23">
         <f>O14/(1-(SUM(N17:N20)))</f>
         <v>1.4492753623188406E-2</v>
       </c>
       <c r="Q24" s="19" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="R24" s="9">
         <f>N48</f>
@@ -3943,7 +3943,7 @@
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B25" s="19" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C25" s="20">
         <f>D18</f>
@@ -3959,14 +3959,14 @@
       </c>
       <c r="F25" s="19"/>
       <c r="H25" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="I25" s="14">
         <f>I18/(1-(I14+I16+I17))</f>
         <v>0.10047846889952154</v>
       </c>
       <c r="M25" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="N25" s="23">
         <f>O15/(1-(SUM(N17:N20)))</f>
@@ -4013,14 +4013,14 @@
         <v>7.1770334928229665E-2</v>
       </c>
       <c r="M26" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="N26" s="23">
         <f>O17/(1-(SUM(N17:N20)))</f>
         <v>0.39130434782608681</v>
       </c>
       <c r="Q26" s="19" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="R26" s="9">
         <f>N51</f>
@@ -4057,7 +4057,7 @@
         <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="N27" s="23">
         <f>O18/(1-(SUM(N17:N20)))</f>
@@ -4082,7 +4082,7 @@
     <row r="28" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B28" s="19"/>
       <c r="C28" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="D28" s="18">
         <f>E24/(1-(D24+D25+D26))</f>
@@ -4091,7 +4091,7 @@
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="M28" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="N28" s="23">
         <f>O19/(1-(SUM(N17:N20)))</f>
@@ -4104,21 +4104,21 @@
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D29" s="18">
         <f>E25/(1-(D24+D25+D26))</f>
         <v>0.36</v>
       </c>
       <c r="M29" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="N29" s="23">
         <f>O20/(1-(SUM(N17:N20)))</f>
         <v>8.6956521739130418E-2</v>
       </c>
       <c r="R29" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="S29" s="35">
         <f>(S15+S18)/(1-(S14+S16+S17+S20+S21+S22+S23+S24+S25+S26))</f>
@@ -4134,20 +4134,20 @@
         <v>0.12</v>
       </c>
       <c r="I30" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="J30" s="19" t="s">
         <v>23</v>
       </c>
       <c r="M30" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="N30" s="23">
         <f>(N14+N21)/(1-(SUM(N17:N20)))</f>
         <v>1.1594202898550723E-2</v>
       </c>
       <c r="R30" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="S30">
         <f>(S19+S27)/(1-(S14+S16+S17+S20+S21+S22+S23+S24+S25+S26))</f>
@@ -4156,7 +4156,7 @@
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D31" s="18">
         <f>D27/(1-(D24+D25+D26))</f>
@@ -4181,7 +4181,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
       <c r="R31" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="S31">
         <f>T14/(1-(S14+S16+S17+S20+S21+S22+S23+S24+S25+S26))</f>
@@ -4197,7 +4197,7 @@
         <v>0.12</v>
       </c>
       <c r="G32" s="19" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="H32" s="6">
         <f>I21</f>
@@ -4216,7 +4216,7 @@
         <v>0.99999999999999967</v>
       </c>
       <c r="R32" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="S32">
         <f>T15/(1-(S14+S16+S17+S20+S21+S22+S23+S24+S25+S26))</f>
@@ -4229,7 +4229,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="19" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="H33" s="6">
         <f>I22</f>
@@ -4244,7 +4244,7 @@
         <v>7.1770334928229665E-2</v>
       </c>
       <c r="R33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="S33">
         <f>T16/(1-(S14+S16+S17+S20+S21+S22+S23+S24+S25+S26))</f>
@@ -4268,7 +4268,7 @@
         <v>2.3923444976076558E-2</v>
       </c>
       <c r="R34" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S34">
         <f>T17/(1-(S14+S16+S17+S20+S21+S22+S23+S24+S25+S26))</f>
@@ -4277,7 +4277,7 @@
     </row>
     <row r="35" spans="4:20" x14ac:dyDescent="0.3">
       <c r="G35" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H35" s="6">
         <f>I24</f>
@@ -4292,13 +4292,13 @@
         <v>7.1770334928229665E-2</v>
       </c>
       <c r="N35" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="O35" s="19" t="s">
         <v>23</v>
       </c>
       <c r="R35" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="S35" s="23">
         <f>T18/(1-(S14+S16+S17+S20+S21+S22+S23+S24+S25+S26))</f>
@@ -4307,7 +4307,7 @@
     </row>
     <row r="36" spans="4:20" x14ac:dyDescent="0.3">
       <c r="G36" s="19" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="H36" s="6">
         <f>I20</f>
@@ -4333,7 +4333,7 @@
         <v>0.58333333333333326</v>
       </c>
       <c r="R36" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="S36" s="23">
         <f>T19/$U$28</f>
@@ -4342,7 +4342,7 @@
     </row>
     <row r="37" spans="4:20" x14ac:dyDescent="0.3">
       <c r="G37" s="19" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="H37" s="6">
         <f>I25</f>
@@ -4357,7 +4357,7 @@
         <v>3.3492822966507185E-2</v>
       </c>
       <c r="L37" s="19" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="M37" s="9">
         <f>N24</f>
@@ -4372,7 +4372,7 @@
         <v>8.4541062801932361E-3</v>
       </c>
       <c r="R37" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="S37" s="23">
         <f t="shared" ref="S37:S44" si="9">T20/$U$28</f>
@@ -4396,7 +4396,7 @@
         <v>2.3923444976076558E-2</v>
       </c>
       <c r="L38" s="19" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="M38" s="9">
         <f>N25</f>
@@ -4411,7 +4411,7 @@
         <v>7.6086956521739121E-2</v>
       </c>
       <c r="R38" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="S38" s="23">
         <f t="shared" si="9"/>
@@ -4435,7 +4435,7 @@
         <v>4.5652173913043465E-2</v>
       </c>
       <c r="R39" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="S39" s="23">
         <f t="shared" si="9"/>
@@ -4444,14 +4444,14 @@
     </row>
     <row r="40" spans="4:20" x14ac:dyDescent="0.3">
       <c r="H40" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="I40" s="32">
         <f>J32/(1-(SUM(I32:I34,I36:I37)))</f>
         <v>1.5197568389057751E-2</v>
       </c>
       <c r="L40" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M40" s="9">
         <f t="shared" ref="M40:M45" si="12">N26</f>
@@ -4466,7 +4466,7 @@
         <v>0.22826086956521727</v>
       </c>
       <c r="R40" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="S40" s="23">
         <f t="shared" si="9"/>
@@ -4476,14 +4476,14 @@
     </row>
     <row r="41" spans="4:20" x14ac:dyDescent="0.3">
       <c r="H41" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="I41">
         <f>J33/(1-(SUM(I32:I34,I36:I37)))</f>
         <v>0.13677811550151975</v>
       </c>
       <c r="L41" s="19" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="M41" s="9">
         <f t="shared" si="12"/>
@@ -4498,7 +4498,7 @@
         <v>0.10652173913043476</v>
       </c>
       <c r="R41" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="S41" s="23">
         <f t="shared" si="9"/>
@@ -4508,14 +4508,14 @@
     </row>
     <row r="42" spans="4:20" x14ac:dyDescent="0.3">
       <c r="H42" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I42">
         <f>J34/(1-(SUM(I32:I34,I36:I37)))</f>
         <v>4.5592705167173259E-2</v>
       </c>
       <c r="L42" s="19" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="M42" s="9">
         <f t="shared" si="12"/>
@@ -4531,7 +4531,7 @@
       </c>
       <c r="Q42" s="7"/>
       <c r="R42" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="S42" s="23">
         <f t="shared" si="9"/>
@@ -4540,14 +4540,14 @@
     </row>
     <row r="43" spans="4:20" x14ac:dyDescent="0.3">
       <c r="H43" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I43">
         <f>(J35+I35)/(1-(SUM(I32:I34,I36:I37)))</f>
         <v>0.41033434650455919</v>
       </c>
       <c r="L43" s="19" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="M43" s="9">
         <f t="shared" si="12"/>
@@ -4563,7 +4563,7 @@
       </c>
       <c r="Q43" s="7"/>
       <c r="R43" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="S43" s="23">
         <f t="shared" si="9"/>
@@ -4572,7 +4572,7 @@
     </row>
     <row r="44" spans="4:20" x14ac:dyDescent="0.3">
       <c r="H44" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="I44">
         <f>J36/(1-(SUM(I32:I34,I36:I37)))</f>
@@ -4604,7 +4604,7 @@
     </row>
     <row r="45" spans="4:20" x14ac:dyDescent="0.3">
       <c r="H45" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="I45">
         <f>J37/(1-(SUM(I32:I34,I36:I37)))</f>
@@ -4633,7 +4633,7 @@
     </row>
     <row r="46" spans="4:20" x14ac:dyDescent="0.3">
       <c r="H46" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="I46">
         <f>I38/(1-(SUM(I32:I34,I36:I37)))</f>
@@ -4652,7 +4652,7 @@
         <v>4.5592705167173259E-2</v>
       </c>
       <c r="M47" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="N47" s="5">
         <f>N37/(1-N40)</f>
@@ -4667,7 +4667,7 @@
         <v>0.99999999999999978</v>
       </c>
       <c r="M48" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="N48">
         <f>N38/(1-N40)</f>
@@ -4679,7 +4679,7 @@
     </row>
     <row r="49" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M49" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="N49" s="5">
         <f>(N39+O39)/((1-N40))</f>
@@ -4691,7 +4691,7 @@
     </row>
     <row r="50" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M50" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="N50" s="5">
         <f>(N42+N41)/(1-N40)</f>
@@ -4703,7 +4703,7 @@
     </row>
     <row r="51" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M51" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="N51" s="5">
         <f>N43/(1-N40)</f>
@@ -4715,7 +4715,7 @@
     </row>
     <row r="52" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M52" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="N52" s="5">
         <f>(N44+O44)/(1-N40)</f>
@@ -4727,7 +4727,7 @@
     </row>
     <row r="53" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M53" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="N53" s="5">
         <f>O37/(1-N40)</f>
@@ -4738,7 +4738,7 @@
     </row>
     <row r="54" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M54" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="N54" s="5">
         <f>O38/(1-N40)</f>
@@ -4747,7 +4747,7 @@
     </row>
     <row r="55" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M55" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="N55" s="5">
         <f>O40/(1-N40)</f>
@@ -4757,7 +4757,7 @@
     </row>
     <row r="56" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M56" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="N56" s="5">
         <f>O41/(1-N40)</f>
@@ -4767,7 +4767,7 @@
     </row>
     <row r="57" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M57" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="N57" s="5">
         <f>O42/(1-N40)</f>
@@ -4777,7 +4777,7 @@
     </row>
     <row r="58" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M58" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="N58">
         <f>O43/(1-N40)</f>
@@ -4787,7 +4787,7 @@
     </row>
     <row r="59" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M59" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="N59">
         <f>N45/(1-N40)</f>

</xml_diff>